<commit_message>
RNN timestep method finished, retrained with the 12 month timestep, started implementing new train/test split
</commit_message>
<xml_diff>
--- a/Metrics/TestingMetrics.xlsx
+++ b/Metrics/TestingMetrics.xlsx
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.254</v>
+        <v>0.276</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.076</v>
+        <v>-0.044</v>
       </c>
       <c r="D3" t="n">
-        <v>0.473</v>
+        <v>0.459</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.677</v>
       </c>
       <c r="F3" t="n">
-        <v>0.783</v>
+        <v>0.768</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.302</v>
+        <v>0.216</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.007</v>
+        <v>-0.131</v>
       </c>
       <c r="D4" t="n">
-        <v>0.443</v>
+        <v>0.498</v>
       </c>
       <c r="E4" t="n">
-        <v>0.666</v>
+        <v>0.706</v>
       </c>
       <c r="F4" t="n">
-        <v>0.726</v>
+        <v>0.744</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.514</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.038</v>
+        <v>-0.004</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.004</v>
+        <v>-0.24</v>
       </c>
       <c r="D5" t="n">
-        <v>0.707</v>
+        <v>0.573</v>
       </c>
       <c r="E5" t="n">
-        <v>0.841</v>
+        <v>0.757</v>
       </c>
       <c r="F5" t="n">
-        <v>0.82</v>
+        <v>0.748</v>
       </c>
       <c r="G5" t="n">
-        <v>0.494</v>
+        <v>0.478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some code rework on desktop
</commit_message>
<xml_diff>
--- a/Metrics/TestingMetrics.xlsx
+++ b/Metrics/TestingMetrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>